<commit_message>
create EnsembleProblem and calculate error with loss function
</commit_message>
<xml_diff>
--- a/data/DataConversion.xlsx
+++ b/data/DataConversion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ferrallm/GitHub/PanCan-PopDynamics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A312D897-C4FB-2346-B630-1A332E226A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBAD457-A2A3-374C-9C59-C2C277652F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25180" yWindow="13600" windowWidth="27240" windowHeight="16440" xr2:uid="{DEDB3298-A5FE-AD4F-881C-E043A9EF7534}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$F$2</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$3:$F$3</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$4:$F$4</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$3:$F$3</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$4:$F$4</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$5:$F$5</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -233,7 +233,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$F$2</c:f>
+              <c:f>Sheet1!$A$3:$F$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -319,7 +319,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$4:$F$4</c:f>
+              <c:f>Sheet1!$A$5:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -405,7 +405,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$F$3</c:f>
+              <c:f>Sheet1!$A$4:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1361,13 +1361,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1693,10 +1693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76CFA66-99D3-2647-92A0-6F8EEC15C618}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1729,102 +1729,71 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
-        <f>I3</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:F2" si="0">J3</f>
-        <v>8839.5540000000001</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <f t="shared" si="0"/>
-        <v>11957.118</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <f t="shared" si="0"/>
-        <v>15204.671999999999</v>
+        <v>18</v>
       </c>
       <c r="E2">
-        <f t="shared" si="0"/>
-        <v>18868.121999999999</v>
+        <v>24</v>
       </c>
       <c r="F2">
-        <f t="shared" si="0"/>
-        <v>23713.937999999998</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1.4732590000000001</v>
-      </c>
-      <c r="K2">
-        <v>1.992853</v>
-      </c>
-      <c r="L2">
-        <v>2.5341119999999999</v>
-      </c>
-      <c r="M2">
-        <v>3.1446869999999998</v>
-      </c>
-      <c r="N2">
-        <v>3.9523229999999998</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f>I6</f>
+        <f>I4</f>
         <v>6000</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:F3" si="1">J6</f>
-        <v>8986.5700799999995</v>
+        <f t="shared" ref="B3:F3" si="0">J4</f>
+        <v>8839.5540000000001</v>
       </c>
       <c r="C3">
-        <f t="shared" si="1"/>
-        <v>12143.741760000001</v>
+        <f t="shared" si="0"/>
+        <v>11957.118</v>
       </c>
       <c r="D3">
-        <f t="shared" si="1"/>
-        <v>15527.800739999999</v>
+        <f t="shared" si="0"/>
+        <v>15204.671999999999</v>
       </c>
       <c r="E3">
-        <f t="shared" si="1"/>
-        <v>19330.04808</v>
+        <f t="shared" si="0"/>
+        <v>18868.121999999999</v>
       </c>
       <c r="F3">
-        <f t="shared" si="1"/>
-        <v>24528.985799999999</v>
-      </c>
-      <c r="I3" s="4">
-        <f>$H$1*I2</f>
-        <v>6000</v>
-      </c>
-      <c r="J3" s="4">
-        <f t="shared" ref="J3:N3" si="2">$H$1*J2</f>
-        <v>8839.5540000000001</v>
-      </c>
-      <c r="K3" s="4">
-        <f t="shared" si="2"/>
-        <v>11957.118</v>
-      </c>
-      <c r="L3" s="4">
-        <f t="shared" si="2"/>
-        <v>15204.671999999999</v>
-      </c>
-      <c r="M3" s="4">
-        <f t="shared" si="2"/>
-        <v>18868.121999999999</v>
-      </c>
-      <c r="N3" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>23713.937999999998</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>11</v>
+      <c r="H3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1.4732590000000001</v>
+      </c>
+      <c r="K3">
+        <v>1.992853</v>
+      </c>
+      <c r="L3">
+        <v>2.5341119999999999</v>
+      </c>
+      <c r="M3">
+        <v>3.1446869999999998</v>
+      </c>
+      <c r="N3">
+        <v>3.9523229999999998</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -1833,134 +1802,187 @@
         <v>6000</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:F4" si="3">J7</f>
+        <f t="shared" ref="B4:F4" si="1">J7</f>
+        <v>8986.5700799999995</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>12143.741760000001</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>15527.800739999999</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>19330.04808</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>24528.985799999999</v>
+      </c>
+      <c r="I4" s="4">
+        <f>$H$1*I3</f>
+        <v>6000</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" ref="J4:N4" si="2">$H$1*J3</f>
+        <v>8839.5540000000001</v>
+      </c>
+      <c r="K4" s="4">
+        <f t="shared" si="2"/>
+        <v>11957.118</v>
+      </c>
+      <c r="L4" s="4">
+        <f t="shared" si="2"/>
+        <v>15204.671999999999</v>
+      </c>
+      <c r="M4" s="4">
+        <f t="shared" si="2"/>
+        <v>18868.121999999999</v>
+      </c>
+      <c r="N4" s="4">
+        <f t="shared" si="2"/>
+        <v>23713.937999999998</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f>I8</f>
+        <v>6000</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:F5" si="3">J8</f>
         <v>8692.5379200000007</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <f t="shared" si="3"/>
         <v>11770.49424</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <f t="shared" si="3"/>
         <v>14881.543259999999</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <f t="shared" si="3"/>
         <v>18406.195919999998</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <f t="shared" si="3"/>
         <v>22898.890199999998</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I4">
+      <c r="I5">
         <v>0</v>
       </c>
-      <c r="J4">
+      <c r="J5">
         <v>2.4502679999999999E-2</v>
       </c>
-      <c r="K4">
+      <c r="K5">
         <v>3.110396E-2</v>
       </c>
-      <c r="L4">
+      <c r="L5">
         <v>5.385479E-2</v>
       </c>
-      <c r="M4">
+      <c r="M5">
         <v>7.6987680000000003E-2</v>
       </c>
-      <c r="N4">
+      <c r="N5">
         <v>0.1358413</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I5">
-        <f>$H$1*I4</f>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <f>$H$1*I5</f>
         <v>0</v>
       </c>
-      <c r="J5">
-        <f t="shared" ref="J5:N5" si="4">$H$1*J4</f>
+      <c r="J6">
+        <f t="shared" ref="J6:N6" si="4">$H$1*J5</f>
         <v>147.01607999999999</v>
       </c>
-      <c r="K5">
+      <c r="K6">
         <f t="shared" si="4"/>
         <v>186.62376</v>
       </c>
-      <c r="L5">
+      <c r="L6">
         <f t="shared" si="4"/>
         <v>323.12873999999999</v>
       </c>
-      <c r="M5">
+      <c r="M6">
         <f t="shared" si="4"/>
         <v>461.92608000000001</v>
       </c>
-      <c r="N5">
+      <c r="N6">
         <f t="shared" si="4"/>
         <v>815.04779999999994</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="4">
-        <f>I3+I5</f>
-        <v>6000</v>
-      </c>
-      <c r="J6" s="4">
-        <f t="shared" ref="J6:N6" si="5">J3+J5</f>
-        <v>8986.5700799999995</v>
-      </c>
-      <c r="K6" s="4">
-        <f t="shared" si="5"/>
-        <v>12143.741760000001</v>
-      </c>
-      <c r="L6" s="4">
-        <f t="shared" si="5"/>
-        <v>15527.800739999999</v>
-      </c>
-      <c r="M6" s="4">
-        <f t="shared" si="5"/>
-        <v>19330.04808</v>
-      </c>
-      <c r="N6" s="4">
-        <f t="shared" si="5"/>
-        <v>24528.985799999999</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="4">
+        <f>I4+I6</f>
+        <v>6000</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" ref="J7:N7" si="5">J4+J6</f>
+        <v>8986.5700799999995</v>
+      </c>
+      <c r="K7" s="4">
+        <f t="shared" si="5"/>
+        <v>12143.741760000001</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="5"/>
+        <v>15527.800739999999</v>
+      </c>
+      <c r="M7" s="4">
+        <f t="shared" si="5"/>
+        <v>19330.04808</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="5"/>
+        <v>24528.985799999999</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="4">
-        <f>I3-I5</f>
+      <c r="I8" s="4">
+        <f>I4-I6</f>
         <v>6000</v>
       </c>
-      <c r="J7" s="4">
-        <f t="shared" ref="J7:N7" si="6">J3-J5</f>
+      <c r="J8" s="4">
+        <f t="shared" ref="J8:N8" si="6">J4-J6</f>
         <v>8692.5379200000007</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K8" s="4">
         <f t="shared" si="6"/>
         <v>11770.49424</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L8" s="4">
         <f t="shared" si="6"/>
         <v>14881.543259999999</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M8" s="4">
         <f t="shared" si="6"/>
         <v>18406.195919999998</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N8" s="4">
         <f t="shared" si="6"/>
         <v>22898.890199999998</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O8" s="4" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>